<commit_message>
Commit fixed BOM and CPS for boot/rest switches.
</commit_message>
<xml_diff>
--- a/CAM_OUTPUTS/PicoBOB_UPLOAD_GERBERS_B1/BOM/PicoBOB_CAM_OUTPUT_B1.xlsx
+++ b/CAM_OUTPUTS/PicoBOB_UPLOAD_GERBERS_B1/BOM/PicoBOB_CAM_OUTPUT_B1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\PicoBOB\Project Outputs for PicoBOB\PicoBOB_UPLOAD_GERBERS_B1\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\PicoBOB\CAM_OUTPUTS\PicoBOB_UPLOAD_GERBERS_B1\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="106">
   <si>
     <t>Comment</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>0805_C</t>
-  </si>
-  <si>
-    <t>C2922481</t>
   </si>
   <si>
     <t>10pF</t>
@@ -354,13 +351,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -404,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -413,6 +416,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,7 +700,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,8 +783,8 @@
       <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
+      <c r="E4" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
@@ -788,19 +792,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
@@ -808,19 +812,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1">
         <v>3</v>
@@ -828,19 +832,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="1">
         <v>5</v>
@@ -848,19 +852,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -868,19 +872,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E9" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -888,19 +892,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -908,19 +912,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
@@ -928,19 +932,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
@@ -948,19 +952,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="F13" s="1">
         <v>12</v>
@@ -968,16 +972,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1">
@@ -986,19 +990,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
@@ -1006,19 +1010,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="F16" s="1">
         <v>2</v>
@@ -1026,19 +1030,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="F17" s="1">
         <v>3</v>
@@ -1046,19 +1050,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="F18" s="1">
         <v>5</v>
@@ -1066,19 +1070,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
@@ -1086,19 +1090,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="F20" s="1">
         <v>17</v>
@@ -1106,19 +1110,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="F21" s="1">
         <v>12</v>
@@ -1126,19 +1130,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="F22" s="1">
         <v>2</v>
@@ -1146,16 +1150,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="D23" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1">
@@ -1164,19 +1168,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
@@ -1184,19 +1188,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
@@ -1204,19 +1208,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Really fixed BOM issue this time.
</commit_message>
<xml_diff>
--- a/CAM_OUTPUTS/PicoBOB_UPLOAD_GERBERS_B1/BOM/PicoBOB_CAM_OUTPUT_B1.xlsx
+++ b/CAM_OUTPUTS/PicoBOB_UPLOAD_GERBERS_B1/BOM/PicoBOB_CAM_OUTPUT_B1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="107">
   <si>
     <t>Comment</t>
   </si>
@@ -345,25 +345,22 @@
   </si>
   <si>
     <t>C77838</t>
+  </si>
+  <si>
+    <t>C129303</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -407,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -416,7 +413,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,7 +696,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,8 +779,8 @@
       <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>40</v>
+      <c r="E4" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>

</xml_diff>